<commit_message>
Add a recursive call example and modify some examples
</commit_message>
<xml_diff>
--- a/example/popcount/popcount1.xlsx
+++ b/example/popcount/popcount1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\verilog\GitHub\StamicCGRA\example\popcount\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C386B74F-B3F3-4910-B562-F48ECD5971AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65FF8C85-8A0E-4695-9699-F4A3B83719F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,14 +25,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>MOV1_2
 (L1,D0,D0)</t>
-  </si>
-  <si>
-    <t>MOV1_2
-(D1,R0,R0)</t>
   </si>
   <si>
     <t>MOV1_2
@@ -98,22 +94,6 @@
   </si>
   <si>
     <t>MOV1_2
-(D1,R0,R0)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>MOV1_2
-(D1,U1,U1)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SWITCH_TAG
-(U1,U0,D0,D1)
-DATA(0x0100)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>MOV1_2
 (R0,U1,U1)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -124,53 +104,13 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>LOOP_HEAD
-(U0,D0,L0,D1)
-DATA(0x4)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>LOOP_HEAD
-(U0,R0,D0,D1)
-DATA(0x4)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>MOV1_2
 (D1,L0,L0)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>MOV1_2
-(L0,U0,U0)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>MOV1_2
-(R0,U0,U0)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ADD_DATA
-(D1,U1)
-DATA(0x1)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>SWITCH_PRED
 (D1,D0,U1,L0)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>MOV1_2
-(D1,U1,U0)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>MOV1_2
-(D1,U1,U1)
-DISCARD
-(D0,D0,D0,D0)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -220,6 +160,41 @@
     <t>MOV1_2
 (L0,R0,R0)
 R0(0x10f)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MOV1_2
+(D1,U0,U0)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DISCARD
+(D0,D0,D0,D0)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADD_DATA
+(D1,U0)
+DATA(0x1)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SWITCH_TAG
+(U0,U1,D0,D1)
+DATA(0x0100)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MOV1_2
+(D0,R0,R0)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>OX(U0,L0,D0)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>OX(U0,R0,D0)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -483,13 +458,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>352425</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>733426</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>352425</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -533,13 +508,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>352426</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -586,13 +561,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>333375</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>333375</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -636,14 +611,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>342900</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>533401</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>533402</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -658,12 +633,15 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="8496300" y="1057275"/>
-          <a:ext cx="0" cy="8763001"/>
+          <a:off x="3295650" y="6438900"/>
+          <a:ext cx="0" cy="3381377"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="1">
@@ -686,13 +664,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>533400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>323851</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>533400</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -736,13 +714,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>314325</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>523876</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -758,12 +736,15 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="6362700" y="1743075"/>
-          <a:ext cx="0" cy="8067676"/>
+          <a:off x="1162050" y="4295775"/>
+          <a:ext cx="0" cy="5514976"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="1">
@@ -787,13 +768,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>428625</xdr:rowOff>
+      <xdr:rowOff>438150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>428625</xdr:rowOff>
+      <xdr:rowOff>438150</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -808,8 +789,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="419100" y="428625"/>
-          <a:ext cx="2085975" cy="0"/>
+          <a:off x="419100" y="1152525"/>
+          <a:ext cx="2143125" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -889,13 +870,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>704850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -942,13 +923,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>323850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>323850</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -992,13 +973,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>333375</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1045,13 +1026,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>333375</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1098,13 +1079,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>704850</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1122,59 +1103,6 @@
         <a:xfrm flipV="1">
           <a:off x="8391525" y="6438900"/>
           <a:ext cx="0" cy="695325"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>333375</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>333375</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="65" name="直線單箭頭接點 64">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98544363-B6DC-41D0-938B-8B1C9BCD4B87}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="8181975" y="1047750"/>
-          <a:ext cx="304800" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1254,13 +1182,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>704850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>695325</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1306,118 +1234,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>314325</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>314325</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="68" name="直線接點 67">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4E01C85-750C-4660-9485-6DEEE42AECB8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6362700" y="1743075"/>
-          <a:ext cx="685800" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>704850</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>304800</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="70" name="直線單箭頭接點 69">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0289405-D1CE-451B-A363-87D2C3AAC9CA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="7048500" y="1419225"/>
-          <a:ext cx="0" cy="314325"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
       <xdr:colOff>276225</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>409575</xdr:rowOff>
+      <xdr:rowOff>295275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1432,8 +1257,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="6219825" y="1123950"/>
-          <a:ext cx="0" cy="1019175"/>
+          <a:off x="1019175" y="1724025"/>
+          <a:ext cx="0" cy="419101"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1461,13 +1286,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>276225</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>419100</xdr:rowOff>
+      <xdr:rowOff>295275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>733425</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>419100</xdr:rowOff>
+      <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1482,214 +1307,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6219825" y="1133475"/>
+          <a:off x="1019175" y="1724025"/>
           <a:ext cx="457200" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>342900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>342900</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="76" name="直線接點 75">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5C21024-532B-4929-BE27-BBA05B61BE70}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6362700" y="4629150"/>
-          <a:ext cx="152400" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>342900</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="78" name="直線單箭頭接點 77">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9754C6F-E12E-4FC8-8294-57C2BCD81B5C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="6515100" y="4295775"/>
-          <a:ext cx="0" cy="333375"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>323850</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>323850</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="80" name="直線接點 79">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF32C063-2408-490D-A385-6CBC03E1880A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8496300" y="6753225"/>
-          <a:ext cx="161925" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>323850</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="81" name="直線單箭頭接點 80">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A53B99CC-3BE5-431D-8E89-DCAEF8FA268B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="8658225" y="6448425"/>
-          <a:ext cx="0" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1719,13 +1338,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>390525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1767,15 +1386,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>390525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>390525</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1791,166 +1410,10 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="7791450" y="1819275"/>
-          <a:ext cx="571500" cy="0"/>
+          <a:off x="2981325" y="1819275"/>
+          <a:ext cx="180975" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>400050</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="87" name="直線單箭頭接點 86">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF7A709B-C1DE-418E-8FC8-36AB5588AE8F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="7791450" y="1428750"/>
-          <a:ext cx="0" cy="400050"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>704850</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="89" name="直線單箭頭接點 88">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17331DE9-1BFA-4DE3-AFD2-9733D298EF33}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7200900" y="1447800"/>
-          <a:ext cx="0" cy="685800"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="91" name="直線單箭頭接點 90">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B08DA47-298E-4A9E-9FD7-0BB5E776B8EB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7591425" y="1438275"/>
-          <a:ext cx="0" cy="704850"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
           <a:avLst/>
         </a:prstGeom>
         <a:ln>
@@ -1978,13 +1441,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>400051</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>400050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>400050</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2327,10 +1790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -2341,212 +1804,191 @@
   <sheetData>
     <row r="1" spans="1:5" ht="56.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="4"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" ht="56.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="56.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="B3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" ht="56.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4"/>
-      <c r="B4" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="B4" s="2"/>
       <c r="C4" s="6" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="56.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="4"/>
-      <c r="B5" s="2" t="s">
-        <v>16</v>
+      <c r="A5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" ht="56.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>26</v>
+      <c r="A6" s="4"/>
+      <c r="B6" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="56.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="56.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
       <c r="B8" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>28</v>
+        <v>4</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="56.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
       <c r="B9" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>29</v>
+        <v>7</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="56.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>27</v>
+        <v>4</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="56.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>5</v>
+        <v>14</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="56.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="B12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>31</v>
+      <c r="C12" s="4"/>
+      <c r="D12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="56.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
       <c r="B13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="2" t="s">
-        <v>32</v>
+      <c r="D13" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="56.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="4"/>
-      <c r="B14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>